<commit_message>
Updated to send it to master
</commit_message>
<xml_diff>
--- a/sheets.xlsx
+++ b/sheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao Lucas\Desktop\get_this_prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{8134AAC8-B8C5-40D1-9C7B-35BF522B2CE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA571BCD-EE2B-4EAF-B598-F98BC0A72A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -90,7 +89,7 @@
     <t>Maior preço</t>
   </si>
   <si>
-    <t>23/out</t>
+    <t>Coluna1</t>
   </si>
 </sst>
 </file>
@@ -508,19 +507,6 @@
   <dxfs count="25">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -857,6 +843,19 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -927,17 +926,17 @@
     <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Produtos" totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="23/out" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="19" dataCellStyle="Hiperlink"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Coluna2" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="17" dataCellStyle="Hiperlink"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Coluna3" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="15" dataCellStyle="Hiperlink"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Coluna4" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="13" dataCellStyle="Hiperlink"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Coluna5" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="11" dataCellStyle="Hiperlink"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Coluna6" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="9" dataCellStyle="Hiperlink"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Coluna7" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="7" dataCellStyle="Hiperlink"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Coluna8" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5" dataCellStyle="Hiperlink"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Coluna9" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="3" dataCellStyle="Hiperlink"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Coluna10" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Hiperlink"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Produtos" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Coluna1" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Coluna2" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Coluna3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Coluna4" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Coluna5" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Coluna6" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Coluna7" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Coluna8" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Coluna9" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Coluna10" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1210,7 +1209,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,9 +1272,7 @@
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="24">
-        <v>1016</v>
-      </c>
+      <c r="B3" s="24"/>
       <c r="C3" s="25"/>
       <c r="D3" s="26"/>
       <c r="E3" s="27"/>
@@ -1290,9 +1287,7 @@
       <c r="A4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="34">
-        <v>600</v>
-      </c>
+      <c r="B4" s="34"/>
       <c r="C4" s="35"/>
       <c r="D4" s="36"/>
       <c r="E4" s="36"/>
@@ -1307,9 +1302,7 @@
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="37">
-        <v>310</v>
-      </c>
+      <c r="B5" s="37"/>
       <c r="C5" s="38"/>
       <c r="D5" s="26"/>
       <c r="E5" s="39"/>
@@ -1324,9 +1317,7 @@
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="37">
-        <v>285</v>
-      </c>
+      <c r="B6" s="37"/>
       <c r="C6" s="38"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
@@ -1341,9 +1332,7 @@
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="37">
-        <v>480</v>
-      </c>
+      <c r="B7" s="37"/>
       <c r="C7" s="38"/>
       <c r="D7" s="26"/>
       <c r="E7" s="27"/>
@@ -1358,9 +1347,7 @@
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="37">
-        <v>520</v>
-      </c>
+      <c r="B8" s="37"/>
       <c r="C8" s="38"/>
       <c r="D8" s="26"/>
       <c r="E8" s="27"/>
@@ -1376,8 +1363,8 @@
         <v>17</v>
       </c>
       <c r="B9" s="40">
-        <f>SUBTOTAL(109,Tabela2[23/out])</f>
-        <v>3211</v>
+        <f>SUBTOTAL(109,Tabela2[Coluna1])</f>
+        <v>0</v>
       </c>
       <c r="C9" s="40">
         <f>SUBTOTAL(109,Tabela2[Coluna2])</f>
@@ -1453,11 +1440,11 @@
       </c>
       <c r="B12" s="42">
         <f>MIN($B$3:$XFD$3)</f>
-        <v>1016</v>
+        <v>0</v>
       </c>
       <c r="C12" s="43">
         <f>MAX($B$3:$XFD$3)</f>
-        <v>1016</v>
+        <v>0</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
@@ -1474,11 +1461,11 @@
       </c>
       <c r="B13" s="42">
         <f>MIN($B$4:$XFD$4)</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="C13" s="43">
         <f>MAX($B$4:$XFD$4)</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="H13" s="17"/>
     </row>
@@ -1488,11 +1475,11 @@
       </c>
       <c r="B14" s="42">
         <f>MIN($B$5:$XFD$5)</f>
-        <v>310</v>
+        <v>0</v>
       </c>
       <c r="C14" s="43">
         <f>MAX($B$5:$XFD$5)</f>
-        <v>310</v>
+        <v>0</v>
       </c>
       <c r="H14" s="17"/>
     </row>
@@ -1502,11 +1489,11 @@
       </c>
       <c r="B15" s="42">
         <f>MIN($B$6:$XFD$6)</f>
-        <v>285</v>
+        <v>0</v>
       </c>
       <c r="C15" s="43">
         <f>MAX($B$6:$XFD$6)</f>
-        <v>285</v>
+        <v>0</v>
       </c>
       <c r="H15" s="17"/>
     </row>
@@ -1516,11 +1503,11 @@
       </c>
       <c r="B16" s="42">
         <f>MIN($B$7:$XFD$7)</f>
-        <v>480</v>
+        <v>0</v>
       </c>
       <c r="C16" s="43">
         <f>MAX($B$7:$XFD$7)</f>
-        <v>480</v>
+        <v>0</v>
       </c>
       <c r="H16" s="17"/>
     </row>
@@ -1530,11 +1517,11 @@
       </c>
       <c r="B17" s="42">
         <f>MIN($B$8:$XFD$8)</f>
-        <v>520</v>
+        <v>0</v>
       </c>
       <c r="C17" s="43">
         <f>MAX($B$8:$XFD$8)</f>
-        <v>520</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
@@ -1543,11 +1530,11 @@
       </c>
       <c r="B18" s="44">
         <f>SUBTOTAL(109,B12:B17)</f>
-        <v>3211</v>
+        <v>0</v>
       </c>
       <c r="C18" s="44">
         <f>SUBTOTAL(109,C12:C17)</f>
-        <v>3211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
🛠 Bug 'index out of range' fixedd
</commit_message>
<xml_diff>
--- a/sheets.xlsx
+++ b/sheets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao Lucas\Desktop\get_this_prices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao Lucas\Desktop\get_this_prices - Copia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA571BCD-EE2B-4EAF-B598-F98BC0A72A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC68A927-52F4-4506-B15C-028EAF51AEA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -89,7 +90,7 @@
     <t>Maior preço</t>
   </si>
   <si>
-    <t>Coluna1</t>
+    <t>23/out</t>
   </si>
 </sst>
 </file>
@@ -526,19 +527,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -558,19 +546,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -590,19 +565,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -622,19 +584,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -654,19 +603,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -686,19 +622,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -718,19 +641,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -750,19 +660,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -782,19 +679,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -814,19 +698,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -843,6 +714,136 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -926,17 +927,17 @@
     <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Produtos" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Coluna1" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Coluna2" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Coluna3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Coluna4" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Coluna5" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Coluna6" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Coluna7" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Coluna8" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Coluna9" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Coluna10" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Produtos" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="23/out" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Coluna2" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Coluna3" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Coluna4" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Coluna5" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Coluna6" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Coluna7" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Coluna8" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Coluna9" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Coluna10" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1209,7 +1210,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,7 +1273,9 @@
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="24"/>
+      <c r="B3" s="24">
+        <v>1054</v>
+      </c>
       <c r="C3" s="25"/>
       <c r="D3" s="26"/>
       <c r="E3" s="27"/>
@@ -1287,7 +1290,9 @@
       <c r="A4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="34">
+        <v>600</v>
+      </c>
       <c r="C4" s="35"/>
       <c r="D4" s="36"/>
       <c r="E4" s="36"/>
@@ -1302,7 +1307,9 @@
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="37"/>
+      <c r="B5" s="37">
+        <v>323</v>
+      </c>
       <c r="C5" s="38"/>
       <c r="D5" s="26"/>
       <c r="E5" s="39"/>
@@ -1317,7 +1324,9 @@
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="37">
+        <v>297</v>
+      </c>
       <c r="C6" s="38"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
@@ -1332,7 +1341,9 @@
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="37">
+        <v>480</v>
+      </c>
       <c r="C7" s="38"/>
       <c r="D7" s="26"/>
       <c r="E7" s="27"/>
@@ -1347,7 +1358,9 @@
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="37">
+        <v>520</v>
+      </c>
       <c r="C8" s="38"/>
       <c r="D8" s="26"/>
       <c r="E8" s="27"/>
@@ -1363,8 +1376,8 @@
         <v>17</v>
       </c>
       <c r="B9" s="40">
-        <f>SUBTOTAL(109,Tabela2[Coluna1])</f>
-        <v>0</v>
+        <f>SUBTOTAL(109,Tabela2[23/out])</f>
+        <v>3274</v>
       </c>
       <c r="C9" s="40">
         <f>SUBTOTAL(109,Tabela2[Coluna2])</f>
@@ -1440,11 +1453,11 @@
       </c>
       <c r="B12" s="42">
         <f>MIN($B$3:$XFD$3)</f>
-        <v>0</v>
+        <v>1054</v>
       </c>
       <c r="C12" s="43">
         <f>MAX($B$3:$XFD$3)</f>
-        <v>0</v>
+        <v>1054</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
@@ -1461,11 +1474,11 @@
       </c>
       <c r="B13" s="42">
         <f>MIN($B$4:$XFD$4)</f>
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="C13" s="43">
         <f>MAX($B$4:$XFD$4)</f>
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="H13" s="17"/>
     </row>
@@ -1475,11 +1488,11 @@
       </c>
       <c r="B14" s="42">
         <f>MIN($B$5:$XFD$5)</f>
-        <v>0</v>
+        <v>323</v>
       </c>
       <c r="C14" s="43">
         <f>MAX($B$5:$XFD$5)</f>
-        <v>0</v>
+        <v>323</v>
       </c>
       <c r="H14" s="17"/>
     </row>
@@ -1489,11 +1502,11 @@
       </c>
       <c r="B15" s="42">
         <f>MIN($B$6:$XFD$6)</f>
-        <v>0</v>
+        <v>297</v>
       </c>
       <c r="C15" s="43">
         <f>MAX($B$6:$XFD$6)</f>
-        <v>0</v>
+        <v>297</v>
       </c>
       <c r="H15" s="17"/>
     </row>
@@ -1503,11 +1516,11 @@
       </c>
       <c r="B16" s="42">
         <f>MIN($B$7:$XFD$7)</f>
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="C16" s="43">
         <f>MAX($B$7:$XFD$7)</f>
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="H16" s="17"/>
     </row>
@@ -1517,11 +1530,11 @@
       </c>
       <c r="B17" s="42">
         <f>MIN($B$8:$XFD$8)</f>
-        <v>0</v>
+        <v>520</v>
       </c>
       <c r="C17" s="43">
         <f>MAX($B$8:$XFD$8)</f>
-        <v>0</v>
+        <v>520</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
@@ -1530,11 +1543,11 @@
       </c>
       <c r="B18" s="44">
         <f>SUBTOTAL(109,B12:B17)</f>
-        <v>0</v>
+        <v>3274</v>
       </c>
       <c r="C18" s="44">
         <f>SUBTOTAL(109,C12:C17)</f>
-        <v>0</v>
+        <v>3274</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Trying to fix ERROR bug
</commit_message>
<xml_diff>
--- a/sheets.xlsx
+++ b/sheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao Lucas\Desktop\get_this_prices - local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{47BEB9DB-6491-42AF-9A15-618EDAC109DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D66A6CC8-99AC-417F-B850-C46FD01D3BB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>Preços do PC</t>
   </si>
@@ -54,6 +54,9 @@
     <t>28/out</t>
   </si>
   <si>
+    <t>29/10</t>
+  </si>
+  <si>
     <t>Coluna8</t>
   </si>
   <si>
@@ -94,9 +97,6 @@
   </si>
   <si>
     <t>Frete</t>
-  </si>
-  <si>
-    <t>29/out</t>
   </si>
 </sst>
 </file>
@@ -251,22 +251,22 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="2" tint="-0.749992370372631"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="10">
@@ -433,7 +433,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -484,7 +484,7 @@
     <xf numFmtId="16" fontId="24" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="26" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="27" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="14" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
@@ -493,7 +493,7 @@
     <xf numFmtId="44" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -506,10 +506,13 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="26" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -518,10 +521,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="28" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Estilo 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -531,14 +530,11 @@
   <dxfs count="25">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -550,14 +546,24 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -569,14 +575,24 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -588,14 +604,24 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -607,14 +633,24 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -626,14 +662,24 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -645,14 +691,24 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -664,14 +720,24 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -683,14 +749,24 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -702,14 +778,24 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -721,152 +807,32 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
       <font>
@@ -950,35 +916,35 @@
     <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Produtos" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="23/out" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Produtos" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="23/out" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
       <totalsRowFormula>SUBTOTAL(109,B3,B5:B8)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="24/out" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="8">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="24/out" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="16">
       <totalsRowFormula>SUBTOTAL(109,C3,C5:C8)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="25/out" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="7">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="25/out" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
       <totalsRowFormula>SUBTOTAL(109,D3,D5:D8)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="26/out" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="6">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="26/out" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12">
       <totalsRowFormula>SUBTOTAL(109,E3,E5:E8)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="27/out" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="5">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="27/out" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <totalsRowFormula>SUBTOTAL(109,F3,F5:F8)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="28/out" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="4">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="28/out" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
       <totalsRowFormula>SUBTOTAL(109,G3,G5:G8)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="29/out" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="3">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="29/out" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
       <totalsRowFormula>SUBTOTAL(109,H3,H5:H8)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Coluna8" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="2">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Coluna8" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
       <totalsRowFormula>SUBTOTAL(109,I3,I5:I8)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Coluna9" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="1">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Coluna9" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
       <totalsRowFormula>SUBTOTAL(109,J3,J5:J8)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Coluna10" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="0">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Coluna10" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
       <totalsRowFormula>SUBTOTAL(109,K3,K5:K8)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1252,8 +1218,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,19 +1229,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
     </row>
     <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1300,21 +1266,21 @@
         <v>7</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="25">
         <v>1054</v>
@@ -1343,7 +1309,7 @@
     </row>
     <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="35">
         <v>600</v>
@@ -1372,7 +1338,7 @@
     </row>
     <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="37">
         <v>323</v>
@@ -1401,7 +1367,7 @@
     </row>
     <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="37">
         <v>297</v>
@@ -1430,7 +1396,7 @@
     </row>
     <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="37">
         <v>480</v>
@@ -1459,7 +1425,7 @@
     </row>
     <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="37">
         <v>520</v>
@@ -1488,7 +1454,7 @@
     </row>
     <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="39">
         <f t="shared" ref="B9:K9" si="0">SUBTOTAL(109,B3,B5:B8)</f>
@@ -1537,8 +1503,8 @@
       <c r="D10" s="40"/>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
       <c r="I10" s="40"/>
       <c r="J10" s="40"/>
       <c r="K10" s="40"/>
@@ -1548,10 +1514,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -1564,13 +1530,13 @@
     </row>
     <row r="12" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="41">
         <f>MIN($B$3:$XFD$3)</f>
         <v>1000</v>
       </c>
-      <c r="C12" s="49">
+      <c r="C12" s="42">
         <f>MAX($B$3:$XFD$3)</f>
         <v>1054</v>
       </c>
@@ -1585,13 +1551,13 @@
     </row>
     <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="41">
         <f>MIN($B$4:$XFD$4)</f>
         <v>600</v>
       </c>
-      <c r="C13" s="49">
+      <c r="C13" s="42">
         <f>MAX($B$4:$XFD$4)</f>
         <v>600</v>
       </c>
@@ -1599,13 +1565,13 @@
     </row>
     <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="41">
         <f>MIN($B$5:$XFD$5)</f>
         <v>290</v>
       </c>
-      <c r="C14" s="49">
+      <c r="C14" s="42">
         <f>MAX($B$5:$XFD$5)</f>
         <v>323</v>
       </c>
@@ -1613,13 +1579,13 @@
     </row>
     <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="41">
         <f>MIN($B$6:$XFD$6)</f>
         <v>260</v>
       </c>
-      <c r="C15" s="49">
+      <c r="C15" s="42">
         <f>MAX($B$6:$XFD$6)</f>
         <v>297</v>
       </c>
@@ -1627,13 +1593,13 @@
     </row>
     <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="41">
         <f>MIN($B$7:$XFD$7)</f>
         <v>420</v>
       </c>
-      <c r="C16" s="49">
+      <c r="C16" s="42">
         <f>MAX($B$7:$XFD$7)</f>
         <v>480</v>
       </c>
@@ -1641,20 +1607,20 @@
     </row>
     <row r="17" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="41">
         <f>MIN($B$8:$XFD$8)</f>
         <v>520</v>
       </c>
-      <c r="C17" s="49">
+      <c r="C17" s="42">
         <f>MAX($B$8:$XFD$8)</f>
         <v>520</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="43">
         <f>SUBTOTAL(109,B12,B14:B17)</f>
@@ -1670,21 +1636,21 @@
         <v>1</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21" s="41">
         <f>SUM(1,-1)</f>
         <v>0</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="44">
         <f>SUM(1,-1)</f>
         <v>0</v>
       </c>
@@ -1692,76 +1658,76 @@
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22" s="41">
         <v>450</v>
       </c>
-      <c r="C22" s="42">
+      <c r="C22" s="44">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23" s="41">
         <f t="shared" ref="B23:C26" si="1">SUM(1,-1)</f>
         <v>0</v>
       </c>
-      <c r="C23" s="42">
+      <c r="C23" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B24" s="41">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C24" s="42">
+      <c r="C24" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B25" s="41">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C25" s="42">
+      <c r="C25" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B26" s="41">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C26" s="42">
+      <c r="C26" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="46">
+        <v>18</v>
+      </c>
+      <c r="B27" s="47">
         <f>SUBTOTAL(109, B21:C26)</f>
         <v>480</v>
       </c>
-      <c r="C27" s="47"/>
+      <c r="C27" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Update just_print to avoid BEING ARRESTED �
</commit_message>
<xml_diff>
--- a/sheets.xlsx
+++ b/sheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao Lucas\Desktop\get_this_prices - local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{003F537B-60D1-404C-9706-11F94BF15C51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{5F15CB3C-B682-4C8A-B1F5-5B0D1D0942CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>02/nov</t>
   </si>
   <si>
-    <t>3/11</t>
-  </si>
-  <si>
     <t>Coluna3</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Grátis</t>
+  </si>
+  <si>
+    <t>03/nov</t>
   </si>
 </sst>
 </file>
@@ -731,11 +731,14 @@
   <dxfs count="55">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -746,15 +749,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -765,15 +768,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -784,15 +787,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -803,15 +806,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -822,15 +825,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -841,15 +844,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -860,15 +863,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -879,15 +882,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -898,15 +901,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -917,15 +920,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -936,15 +939,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -955,15 +958,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -974,15 +977,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -993,15 +996,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -1012,15 +1015,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -1031,15 +1034,15 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -1051,25 +1054,14 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -1081,25 +1073,14 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -1111,25 +1092,14 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -1141,25 +1111,14 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -1171,25 +1130,14 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -1201,25 +1149,14 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -1231,25 +1168,14 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -1261,25 +1187,14 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
@@ -1291,33 +1206,196 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center"/>
     </dxf>
     <dxf>
       <font>
@@ -1416,80 +1494,80 @@
     <filterColumn colId="25" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Produtos" totalsRowLabel="Total" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="23/out" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="48">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Produtos" totalsRowLabel="Total" dataDxfId="51" totalsRowDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="23/out" totalsRowFunction="custom" dataDxfId="50" totalsRowDxfId="24">
       <totalsRowFormula>SUBTOTAL(109,B3,B6:B10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="24/out" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="46">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="24/out" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="23">
       <totalsRowFormula>SUBTOTAL(109,C3,C6:C10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="25/out" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="44">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="25/out" totalsRowFunction="custom" dataDxfId="48" totalsRowDxfId="22">
       <totalsRowFormula>SUBTOTAL(109,D3,D6:D10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="26/out" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="42">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="26/out" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="21">
       <totalsRowFormula>SUBTOTAL(109,E3,E6:E10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="27/out" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="40">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="27/out" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="20">
       <totalsRowFormula>SUBTOTAL(109,F3,F6:F10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="28/out" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="38">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="28/out" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="19">
       <totalsRowFormula>SUBTOTAL(109,G3,G6:G10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="29/out" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="36">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="29/out" totalsRowFunction="custom" dataDxfId="44" totalsRowDxfId="18">
       <totalsRowFormula>SUBTOTAL(109,H3,H6:H10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="30/out" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="34">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="30/out" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="17">
       <totalsRowFormula>SUBTOTAL(109,I3,I6:I10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="31/out" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="32">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="31/out" totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="16">
       <totalsRowFormula>SUBTOTAL(109,J3,J6:J10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="01/nov" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="30">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="01/nov" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="15">
       <totalsRowFormula>SUBTOTAL(109,K3,K6:K10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="02/nov" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="02/nov" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="14">
       <totalsRowFormula>SUBTOTAL(109,L3,L6:L10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="03/nov" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="26">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="03/nov" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="13">
       <totalsRowFormula>SUBTOTAL(109,M3,M6:M10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Coluna3" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="24">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Coluna3" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="12">
       <totalsRowFormula>SUBTOTAL(109,N3,N6:N10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Coluna4" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Coluna4" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="11">
       <totalsRowFormula>SUBTOTAL(109,O3,O6:O10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Coluna5" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Coluna5" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="10">
       <totalsRowFormula>SUBTOTAL(109,P3,P6:P10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Coluna6" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Coluna6" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="9">
       <totalsRowFormula>SUBTOTAL(109,Q3,Q6:Q10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Coluna7" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="16">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Coluna7" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="8">
       <totalsRowFormula>SUBTOTAL(109,R3,R6:R10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Coluna8" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Coluna8" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="7">
       <totalsRowFormula>SUBTOTAL(109,S3,S6:S10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Coluna9" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Coluna9" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="6">
       <totalsRowFormula>SUBTOTAL(109,T3,T6:T10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Coluna10" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Coluna10" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="5">
       <totalsRowFormula>SUBTOTAL(109,U3,U6:U10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Coluna11" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Coluna11" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="4">
       <totalsRowFormula>SUBTOTAL(109,V3,V6:V10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Coluna12" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Coluna12" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="3">
       <totalsRowFormula>SUBTOTAL(109,W3,W6:W10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Coluna13" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Coluna13" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="2">
       <totalsRowFormula>SUBTOTAL(109,X3,X6:X10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Coluna14" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Coluna14" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="1">
       <totalsRowFormula>SUBTOTAL(109,Y3,Y6:Y10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Coluna15" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Coluna15" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="0">
       <totalsRowFormula>SUBTOTAL(109,Z3,Z6:Z10)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1763,8 +1841,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:AG33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,51 +1926,51 @@
         <v>12</v>
       </c>
       <c r="M2" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="36">
         <v>1054</v>
@@ -1946,7 +2024,7 @@
     </row>
     <row r="4" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="21">
         <v>600</v>
@@ -2000,7 +2078,7 @@
     </row>
     <row r="5" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="48">
         <v>323</v>
@@ -2054,7 +2132,7 @@
     </row>
     <row r="6" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="49">
         <v>297</v>
@@ -2108,7 +2186,7 @@
     </row>
     <row r="7" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="51">
         <v>480</v>
@@ -2162,7 +2240,7 @@
     </row>
     <row r="8" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="51">
         <v>520</v>
@@ -2216,7 +2294,7 @@
     </row>
     <row r="9" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="51">
         <v>76</v>
@@ -2270,7 +2348,7 @@
     </row>
     <row r="10" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="31">
         <v>495</v>
@@ -2324,7 +2402,7 @@
     </row>
     <row r="11" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="53">
         <f t="shared" ref="B11:Z11" si="0">SUBTOTAL(109,B3,B6:B10)</f>
@@ -2442,16 +2520,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="54">
         <f>MIN($B$3:$XFD$3)</f>
@@ -2465,7 +2543,7 @@
     </row>
     <row r="15" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="54">
         <f>MIN($B$4:$XFD$4)</f>
@@ -2479,7 +2557,7 @@
     </row>
     <row r="16" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="54">
         <f>MIN($B$5:$XFD$5)</f>
@@ -2493,7 +2571,7 @@
     </row>
     <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="54">
         <f>MIN($B$6:$XFD$6)</f>
@@ -2506,7 +2584,7 @@
     </row>
     <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="54">
         <f>MIN($B$7:$XFD$7)</f>
@@ -2519,7 +2597,7 @@
     </row>
     <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="54">
         <f>MIN($B$8:$XFD$8)</f>
@@ -2532,7 +2610,7 @@
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="54">
         <f>MIN($B$9:$XFD$9)</f>
@@ -2545,7 +2623,7 @@
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="54">
         <f>MIN($B$10:$XFD$10)</f>
@@ -2559,7 +2637,7 @@
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="56">
         <f>SUBTOTAL(109,B14,B17:B20)</f>
@@ -2576,15 +2654,15 @@
         <v>1</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="54">
         <f>SUM(1,-1)</f>
@@ -2597,7 +2675,7 @@
     </row>
     <row r="26" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="54">
         <v>450</v>
@@ -2608,18 +2686,18 @@
     </row>
     <row r="27" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="59" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="54">
         <f t="shared" ref="B28:C32" si="1">SUM(1,-1)</f>
@@ -2632,7 +2710,7 @@
     </row>
     <row r="29" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="54">
         <f t="shared" si="1"/>
@@ -2645,7 +2723,7 @@
     </row>
     <row r="30" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="54">
         <f t="shared" si="1"/>
@@ -2658,7 +2736,7 @@
     </row>
     <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="54">
         <f t="shared" si="1"/>
@@ -2671,7 +2749,7 @@
     </row>
     <row r="32" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="54">
         <f t="shared" si="1"/>
@@ -2684,7 +2762,7 @@
     </row>
     <row r="33" spans="1:3" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" s="62">
         <f>SUBTOTAL(109, B25:C32)</f>

</xml_diff>

<commit_message>
🚀 Change names in spreadsheet and add screenshot
</commit_message>
<xml_diff>
--- a/sheets.xlsx
+++ b/sheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao Lucas\Desktop\get_this_prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA571BCD-EE2B-4EAF-B598-F98BC0A72A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47B579C-5140-4B0C-9748-8B7CD88A13FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,51 +35,6 @@
     <t>Produtos</t>
   </si>
   <si>
-    <t>Coluna2</t>
-  </si>
-  <si>
-    <t>Coluna3</t>
-  </si>
-  <si>
-    <t>Coluna4</t>
-  </si>
-  <si>
-    <t>Coluna5</t>
-  </si>
-  <si>
-    <t>Coluna6</t>
-  </si>
-  <si>
-    <t>Coluna7</t>
-  </si>
-  <si>
-    <t>Coluna8</t>
-  </si>
-  <si>
-    <t>Coluna9</t>
-  </si>
-  <si>
-    <t>Coluna10</t>
-  </si>
-  <si>
-    <t>Processador AMD Ryzen 5 3400G</t>
-  </si>
-  <si>
-    <t>Placa-Mãe Asus EX-A320M-Gaming</t>
-  </si>
-  <si>
-    <t>HD Seagate BarraCuda, 1TB</t>
-  </si>
-  <si>
-    <t>Memória HyperX Fury 8GB</t>
-  </si>
-  <si>
-    <t>Fonte Corsair 450W 80 Plus Bronze</t>
-  </si>
-  <si>
-    <t>Gabinete Gamer NOX, RGB Rainbow</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -89,7 +44,52 @@
     <t>Maior preço</t>
   </si>
   <si>
-    <t>Coluna1</t>
+    <t>Exemplo de produto 1</t>
+  </si>
+  <si>
+    <t>Exemplo de produto 2</t>
+  </si>
+  <si>
+    <t>Exemplo de produto 3</t>
+  </si>
+  <si>
+    <t>Exemplo de produto 4</t>
+  </si>
+  <si>
+    <t>Exemplo de produto 5</t>
+  </si>
+  <si>
+    <t>Exemplo de produto 6</t>
+  </si>
+  <si>
+    <t>01/jan</t>
+  </si>
+  <si>
+    <t>02/jan</t>
+  </si>
+  <si>
+    <t>03/jan</t>
+  </si>
+  <si>
+    <t>04/jan</t>
+  </si>
+  <si>
+    <t>05/jan</t>
+  </si>
+  <si>
+    <t>06/jan</t>
+  </si>
+  <si>
+    <t>07/jan</t>
+  </si>
+  <si>
+    <t>08/jan</t>
+  </si>
+  <si>
+    <t>09/jan</t>
+  </si>
+  <si>
+    <t>10/jan</t>
   </si>
 </sst>
 </file>
@@ -100,7 +100,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,7 +137,7 @@
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -147,8 +147,9 @@
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -159,7 +160,6 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -168,7 +168,17 @@
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -183,8 +193,8 @@
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -202,60 +212,10 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="9">
@@ -416,7 +376,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -433,60 +393,34 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="21" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="24" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="27" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="28" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="25" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="28" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="25" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="23" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="17" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="16" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -526,19 +460,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -558,19 +479,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -590,19 +498,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -622,19 +517,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -654,19 +536,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -686,19 +555,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -718,19 +574,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -750,19 +593,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -782,19 +612,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -814,19 +631,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -843,6 +647,136 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -926,17 +860,17 @@
     <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Produtos" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Coluna1" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Coluna2" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Coluna3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Coluna4" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Coluna5" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Coluna6" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Coluna7" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Coluna8" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Coluna9" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Coluna10" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Produtos" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="01/jan" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="02/jan" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="03/jan" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="04/jan" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="05/jan" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="06/jan" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="07/jan" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="08/jan" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="09/jan" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="10/jan" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1208,338 +1142,338 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="15.7109375" style="20" customWidth="1"/>
+    <col min="1" max="1" width="41.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="15.7109375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
     </row>
     <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="33"/>
+        <v>5</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="33"/>
+        <v>7</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="23"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="33"/>
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33"/>
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="23"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33"/>
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="23"/>
     </row>
     <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="40">
-        <f>SUBTOTAL(109,Tabela2[Coluna1])</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="40">
-        <f>SUBTOTAL(109,Tabela2[Coluna2])</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="40">
-        <f>SUBTOTAL(109,Tabela2[Coluna3])</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="40">
-        <f>SUBTOTAL(109,Tabela2[Coluna4])</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="40">
-        <f>SUBTOTAL(109,Tabela2[Coluna5])</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="40">
-        <f>SUBTOTAL(109,Tabela2[Coluna6])</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="40">
-        <f>SUBTOTAL(109,Tabela2[Coluna7])</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="40">
-        <f>SUBTOTAL(109,Tabela2[Coluna8])</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="40">
-        <f>SUBTOTAL(109,Tabela2[Coluna9])</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="40">
-        <f>SUBTOTAL(109,Tabela2[Coluna10])</f>
+        <v>2</v>
+      </c>
+      <c r="B9" s="30">
+        <f>SUBTOTAL(109,Tabela2[01/jan])</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="30">
+        <f>SUBTOTAL(109,Tabela2[02/jan])</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="30">
+        <f>SUBTOTAL(109,Tabela2[03/jan])</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="30">
+        <f>SUBTOTAL(109,Tabela2[04/jan])</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="30">
+        <f>SUBTOTAL(109,Tabela2[05/jan])</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="30">
+        <f>SUBTOTAL(109,Tabela2[06/jan])</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="30">
+        <f>SUBTOTAL(109,Tabela2[07/jan])</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="30">
+        <f>SUBTOTAL(109,Tabela2[08/jan])</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="30">
+        <f>SUBTOTAL(109,Tabela2[09/jan])</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="30">
+        <f>SUBTOTAL(109,Tabela2[10/jan])</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="42">
+        <v>5</v>
+      </c>
+      <c r="B12" s="32">
         <f>MIN($B$3:$XFD$3)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="33">
         <f>MAX($B$3:$XFD$3)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="42">
+      <c r="A13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="32">
         <f>MIN($B$4:$XFD$4)</f>
         <v>0</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="33">
         <f>MAX($B$4:$XFD$4)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="17"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="42">
+        <v>7</v>
+      </c>
+      <c r="B14" s="32">
         <f>MIN($B$5:$XFD$5)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="33">
         <f>MAX($B$5:$XFD$5)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="17"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="42">
+        <v>8</v>
+      </c>
+      <c r="B15" s="32">
         <f>MIN($B$6:$XFD$6)</f>
         <v>0</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="33">
         <f>MAX($B$6:$XFD$6)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="17"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="42">
+        <v>9</v>
+      </c>
+      <c r="B16" s="32">
         <f>MIN($B$7:$XFD$7)</f>
         <v>0</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="33">
         <f>MAX($B$7:$XFD$7)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="17"/>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="42">
+        <v>10</v>
+      </c>
+      <c r="B17" s="32">
         <f>MIN($B$8:$XFD$8)</f>
         <v>0</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="33">
         <f>MAX($B$8:$XFD$8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="44">
+        <v>2</v>
+      </c>
+      <c r="B18" s="34">
         <f>SUBTOTAL(109,B12:B17)</f>
         <v>0</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="34">
         <f>SUBTOTAL(109,C12:C17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="11"/>
+      <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1551,6 +1485,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
   </mergeCells>
+  <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="B3:H3">
     <cfRule type="colorScale" priority="11">
       <colorScale>
@@ -1684,9 +1619,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>